<commit_message>
added a new instruction encoding
</commit_message>
<xml_diff>
--- a/documentation/Instruction_Encodings.xlsx
+++ b/documentation/Instruction_Encodings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/James/Library/Mobile Documents/com~apple~CloudDocs/James's Files/Education/Syracuse/Semesters/October 2021/CIS 655 - Advanced computer architecture/HW2/VLQRISC_Simulator/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{400602EF-D045-D448-B175-B18D397CF699}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4541205-9600-5647-910A-B5A7AD48F40C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{8D9666D9-516F-FF40-B233-BE68FB4D243F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
   <si>
     <t>opcode</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>GPR_NUM</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>COMP_BRANCH</t>
   </si>
 </sst>
 </file>
@@ -523,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AE561F5-11A4-7B43-84EF-DCBF10B4A450}">
-  <dimension ref="A1:AG4"/>
+  <dimension ref="A1:AG6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -756,9 +762,64 @@
       <c r="AF4" s="9"/>
       <c r="AG4" s="10"/>
     </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="9"/>
+      <c r="Y6" s="9"/>
+      <c r="Z6" s="9"/>
+      <c r="AA6" s="9"/>
+      <c r="AB6" s="9"/>
+      <c r="AC6" s="9"/>
+      <c r="AD6" s="9"/>
+      <c r="AE6" s="9"/>
+      <c r="AF6" s="9"/>
+      <c r="AG6" s="10"/>
+    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="13">
     <mergeCell ref="O4:AG4"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="G6:J6"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="R6:AG6"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="G2:J2"/>
     <mergeCell ref="K2:N2"/>

</xml_diff>